<commit_message>
Newest Version in 05.15-4
</commit_message>
<xml_diff>
--- a/Assets/course_spreadsheet.xlsx
+++ b/Assets/course_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Map-My-Major\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5EEAC1-244C-447C-AC04-DE42E1BE4058}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AFB5A7-5B75-4214-AB9A-7B81420AB1D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="7035" tabRatio="993" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="7035" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATHSTATS" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="88">
   <si>
     <t>Course:</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>CSC/CYEN 132, MATH 240</t>
-  </si>
-  <si>
-    <t>CSC 132, MATH 240</t>
   </si>
 </sst>
 </file>
@@ -810,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="A1:D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -979,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1447,7 +1444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>

</xml_diff>